<commit_message>
catalogo de cuentas con id
</commit_message>
<xml_diff>
--- a/PLANTILLAS PARA IMPORTACION/CUENTAS POR COBRAR/CLIENTES/res.parter.template.WORKING.xlsx
+++ b/PLANTILLAS PARA IMPORTACION/CUENTAS POR COBRAR/CLIENTES/res.parter.template.WORKING.xlsx
@@ -5,15 +5,16 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="980" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Sheet 1'!$E$1:$E$695</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Sheet 1'!$A$91:$F$695</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Sheet 1'!$E$1:$E$695</definedName>
+    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Sheet 1'!$A$91:$F$695</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Sheet 1'!$E$1:$E$695</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">'Sheet 1'!$A$91:$F$695</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">'Sheet 1'!$E$1:$E$695</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -6724,6 +6725,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -6745,12 +6747,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -6882,37 +6886,38 @@
   <dimension ref="A1:AI695"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="B4" activeCellId="0" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.20918367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="48.5969387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="51.1632653061225"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.7908163265306"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="56.0204081632653"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="42.6581632653061"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="30.2397959183673"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="43.3316326530612"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="30.2397959183673"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="17.0102040816327"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="30.2397959183673"/>
-    <col collapsed="false" hidden="false" max="21" min="19" style="0" width="32.530612244898"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="42.9285714285714"/>
-    <col collapsed="false" hidden="false" max="27" min="23" style="0" width="30.2397959183673"/>
-    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="45.8979591836735"/>
-    <col collapsed="false" hidden="false" max="36" min="29" style="0" width="30.2397959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="37" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="6.0765306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="47.9234693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="50.484693877551"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="42.3877551020408"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="55.3469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="42.25"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="42.7908163265306"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="0" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="16.7397959183673"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="6.75"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="21" min="19" style="0" width="32.1275510204082"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="0" width="42.3877551020408"/>
+    <col collapsed="false" hidden="false" max="27" min="23" style="0" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="0" width="45.3571428571429"/>
+    <col collapsed="false" hidden="false" max="36" min="29" style="0" width="29.8316326530612"/>
+    <col collapsed="false" hidden="false" max="1025" min="37" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -27736,7 +27741,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="E1:E695"/>
+  <autoFilter ref="A91:F695"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="false"/>
   <pageMargins left="0.3" right="0.3" top="0.609722222222222" bottom="0.370138888888889" header="0.1" footer="0.1"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="overThenDown" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>